<commit_message>
filtering excel book rows
</commit_message>
<xml_diff>
--- a/xls/FreeEnglishTextbooks.xlsx
+++ b/xls/FreeEnglishTextbooks.xlsx
@@ -8,23 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markuvinicius/Documents/Workspace/SpringlerBooks/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318EBF60-E5C6-4042-9FA5-99F7F88E6805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC09379-1594-7941-B0FB-48B6EBEA9756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
-    <sheet name="eBook list" sheetId="1" r:id="rId2"/>
+    <sheet name="eBook list" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'eBook list'!$A$1:$V$410</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'eBook list'!$A$1:$V$410</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9074" uniqueCount="3209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8611" uniqueCount="3209">
   <si>
     <t>Book Title</t>
   </si>
@@ -10010,1545 +10009,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55638B8-6F4D-C84F-BEC4-F923AAEECB4F}">
-  <dimension ref="A1:V22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="60" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="86.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="57.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="232.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>2776</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2777</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>2778</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>2779</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>2780</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>2781</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>2782</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>2783</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2784</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2364</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>2785</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>2786</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>2787</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>2788</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>2789</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2803</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>2804</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2805</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>968</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>2806</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>2807</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>2808</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>2809</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>2810</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>2811</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>2812</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>2679</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>2813</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>2814</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>2815</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>2816</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>2817</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>2818</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>2819</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>2820</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>2821</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>2822</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>2823</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>2824</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>2834</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>2835</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>2488</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>2836</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>2837</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>2673</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>2674</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>2838</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>2839</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>2840</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>2841</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>2842</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>2843</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>2844</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>2852</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>2853</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>2364</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>2854</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>2855</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>2856</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>2857</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>2858</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>2859</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>2860</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>2679</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>2861</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>2862</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>2863</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>2864</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>2865</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V9" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>2873</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>2874</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>2875</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>2876</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>2877</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>2878</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>2879</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>2880</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>2881</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>2488</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>2341</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>2882</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>2883</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>2673</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>2674</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>1745</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>1746</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>1747</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>2884</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>2885</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>2886</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="V11" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>2887</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>2881</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>2488</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>2341</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>2888</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>2889</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>2673</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>2674</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>1745</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>1746</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>1747</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>2890</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>2891</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>2886</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="V12" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>2899</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>2900</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>2488</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>933</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>2901</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>2902</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>2673</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>2674</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>1745</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>1746</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>1747</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>2903</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>2904</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>2905</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V13" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>2920</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>2921</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>2922</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>2923</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>2924</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>2925</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>2926</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V14" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>2969</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>2970</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>2679</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>2971</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>2972</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>2973</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>2974</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>2975</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V15" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>2981</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>2982</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>2750</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>2983</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>2984</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>917</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>918</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>919</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>2985</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>2986</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>2987</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>3069</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>3070</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>2488</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>3071</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>3072</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>3073</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>3074</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>3075</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>3076</v>
-      </c>
-      <c r="S17" s="2" t="s">
-        <v>3077</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>3078</v>
-      </c>
-      <c r="U17" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V17" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>3097</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>3098</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>2488</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>3099</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>3100</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>3101</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>3102</v>
-      </c>
-      <c r="T18" s="2" t="s">
-        <v>3103</v>
-      </c>
-      <c r="U18" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V18" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>3142</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>3143</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>2488</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>3144</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>3145</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>3146</v>
-      </c>
-      <c r="R19" s="2" t="s">
-        <v>3147</v>
-      </c>
-      <c r="S19" s="2" t="s">
-        <v>3148</v>
-      </c>
-      <c r="T19" s="2" t="s">
-        <v>3149</v>
-      </c>
-      <c r="U19" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V19" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>3157</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>3158</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>3129</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="1">
-        <v>2020</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>2341</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>3159</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>3160</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>2673</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>2674</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>3161</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>3162</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>3163</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="R20" s="2" t="s">
-        <v>3164</v>
-      </c>
-      <c r="S20" s="2" t="s">
-        <v>3165</v>
-      </c>
-      <c r="T20" s="2" t="s">
-        <v>3166</v>
-      </c>
-      <c r="U20" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="V20" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>3174</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>2470</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>2488</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>3175</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>3176</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>3177</v>
-      </c>
-      <c r="S21" s="2" t="s">
-        <v>3178</v>
-      </c>
-      <c r="T21" s="2" t="s">
-        <v>3179</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V21" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>3180</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>2470</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>2488</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>3181</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>3182</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>3183</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>3184</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>3179</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="V22" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:V410"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S272" sqref="S272"/>
     </sheetView>

</xml_diff>